<commit_message>
Update TendencyData System (Not Json)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage1/Beach.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage1/Beach.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D963723-2325-4D39-B965-D81DDA74EB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2F23CB-0C98-4ECA-A5EF-6CBA7F4F55FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="655" activeTab="2" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
@@ -3801,7 +3801,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="86">
   <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4104,15 +4104,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>(발로 찬다.)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>(머리를 쓰다듬는다.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>열쇠 &lt;b&gt;&lt;극단&gt;&lt;/b&gt;을 획득하였다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,0,1,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,0,2,0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5094,8 +5102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C200D7-C0B4-4460-8B8F-6B50F370EC7E}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -5428,7 +5436,7 @@
     <row r="22" spans="1:6">
       <c r="A22" s="7"/>
       <c r="B22" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" s="7">
         <v>2</v>
@@ -5449,12 +5457,14 @@
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="7"/>
       <c r="B24" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="7">
         <v>2</v>
@@ -5468,14 +5478,16 @@
         <v>26</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C25" s="7">
         <v>1</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="7"/>

</xml_diff>

<commit_message>
Update TendencyData System (Not Json) (#78)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage1/Beach.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage1/Beach.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D963723-2325-4D39-B965-D81DDA74EB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2F23CB-0C98-4ECA-A5EF-6CBA7F4F55FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="655" activeTab="2" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
@@ -3801,7 +3801,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="86">
   <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4104,15 +4104,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>(발로 찬다.)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>(머리를 쓰다듬는다.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>열쇠 &lt;b&gt;&lt;극단&gt;&lt;/b&gt;을 획득하였다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,0,1,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,0,2,0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5094,8 +5102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C200D7-C0B4-4460-8B8F-6B50F370EC7E}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -5428,7 +5436,7 @@
     <row r="22" spans="1:6">
       <c r="A22" s="7"/>
       <c r="B22" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" s="7">
         <v>2</v>
@@ -5449,12 +5457,14 @@
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="7"/>
       <c r="B24" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="7">
         <v>2</v>
@@ -5468,14 +5478,16 @@
         <v>26</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C25" s="7">
         <v>1</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="7"/>

</xml_diff>

<commit_message>
Update TendencyData System (Not Json) - Fix Excel (#78)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage1/Beach.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage1/Beach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2F23CB-0C98-4ECA-A5EF-6CBA7F4F55FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE635A1-6DAB-44E9-A219-BD6A9E686540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="655" activeTab="2" xr2:uid="{8980CEE3-478D-4723-BEB1-C8C193204C53}"/>
   </bookViews>
@@ -5102,8 +5102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C200D7-C0B4-4460-8B8F-6B50F370EC7E}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -5443,7 +5443,9 @@
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="7" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="7" t="s">
@@ -5457,9 +5459,7 @@
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="7" t="s">
-        <v>84</v>
-      </c>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="7"/>
@@ -5471,7 +5471,9 @@
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="F24" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="7" t="s">
@@ -5485,9 +5487,7 @@
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="7" t="s">
-        <v>85</v>
-      </c>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="7"/>

</xml_diff>

<commit_message>
Update UI & Necklace Tendency word UI
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage1/Beach.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage1/Beach.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B9BB5D-75F2-44FF-8E83-815B3018BBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="!Sample" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="1-3 main-0" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="1-3 main-1" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="1-3, 1" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="1-3, 2" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="1-3, 3" sheetId="6" r:id="rId9"/>
+    <sheet name="!Sample" sheetId="1" r:id="rId1"/>
+    <sheet name="1-3 main-0" sheetId="2" r:id="rId2"/>
+    <sheet name="1-3 main-1" sheetId="3" r:id="rId3"/>
+    <sheet name="1-3, 1" sheetId="4" r:id="rId4"/>
+    <sheet name="1-3, 2" sheetId="5" r:id="rId5"/>
+    <sheet name="1-3, 3" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="z+DT7o7porseD4XXZZXxVcYexPRtbcPrOX3Ci11Z6AE="/>
@@ -21,14 +30,74 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="E4">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRk
+UISU    (2023-06-16 00:11:14)
+0: NONE
+1: 대화
+2: 선택지 (1, 2, 3)
+3: 선택지 종료
+4: 맵 이동 (이동할 Scene 이름 - contents)
+5: Save
+9: Random
+10: Random End
+11: Immediately Execute
+// Inspector창에서 직접 조정
+6: CutScene
+7: WaitInteract
+8: Interact</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRc
+UISU    (2023-06-16 00:11:14)
+Dubby = -1,
+    Keep = 0,
+    None = 1,
+    Protagonist = 2,
+    Naru = 3,
+    Photographer = 4,
+    Doctor = 5,
+    Dog = 6,
+    PhotographerSon = 7,
+    PhotographerWife = 8,</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSU
 UISU    (2023-06-16 00:11:14)
 Default = -1
@@ -36,11 +105,19 @@
 Action1 = 1
 …
 Option에서 Left or Right 필수</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="F4">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSA
 서 의수    (2023-06-16 00:11:14)
 이미 사용하고 있는 구분자
@@ -62,12 +139,35 @@
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
 v2 - true, false 다음 Index로 Auto 여부 (Default - true)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="C4">
+  </commentList>
+  <extLst>
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjK335ix46titMzMPgIl0zgeEef9Q=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRk
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRg
 UISU    (2023-06-16 00:11:14)
 0: NONE
 1: 대화
@@ -82,43 +182,19 @@
 6: CutScene
 7: WaitInteract
 8: Interact</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="D4">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRc
-UISU    (2023-06-16 00:11:14)
-Dubby = -1,
-    Keep = 0,
-    None = 1,
-    Protagonist = 2,
-    Naru = 3,
-    Photographer = 4,
-    Doctor = 5,
-    Dog = 6,
-    PhotographerSon = 7,
-    PhotographerWife = 8,</t>
-      </text>
-    </comment>
-  </commentList>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjK335ix46titMzMPgIl0zgeEef9Q=="/>
-    </ext>
-  </extLst>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="D4">
-      <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSs
 UISU    (2023-06-16 00:11:14)
 Dubby = -1,
@@ -131,11 +207,39 @@
     Dog = 6,
     PhotographerSon = 7,
     PhotographerWife = 8,</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="F4">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbSY
+UISU    (2023-06-16 00:11:14)
+Default = -1
+Keep = 0 (이전 유지), (기본)
+Action1 = 1
+…
+Option에서 Left or Right 필수</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSk
 서 의수    (2023-06-16 00:11:14)
 이미 사용하고 있는 구분자
@@ -157,24 +261,35 @@
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
 v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="E4">
+  </commentList>
+  <extLst>
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgJDK4yi5U9B8/yWEBOphYrXagDfQ=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbSY
-UISU    (2023-06-16 00:11:14)
-Default = -1
-Keep = 0 (이전 유지), (기본)
-Action1 = 1
-…
-Option에서 Left or Right 필수</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="C4">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRg
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbSc
 UISU    (2023-06-16 00:11:14)
 0: NONE
 1: 대화
@@ -189,26 +304,64 @@
 6: CutScene
 7: WaitInteract
 8: Interact</t>
+        </r>
       </text>
     </comment>
-  </commentList>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgJDK4yi5U9B8/yWEBOphYrXagDfQ=="/>
-    </ext>
-  </extLst>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="F4">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRY
+UISU    (2023-06-16 00:11:14)
+Dubby = -1,
+    Keep = 0,
+    None = 1,
+    Protagonist = 2,
+    Naru = 3,
+    Photographer = 4,
+    Doctor = 5,
+    Dog = 6,
+    PhotographerSon = 7,
+    PhotographerWife = 8,</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbR0
+UISU    (2023-06-16 00:11:14)
+Default = -1
+Keep = 0 (이전 유지), (기본)
+Action1 = 1
+…
+Option에서 Left or Right 필수</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSg
 서 의수    (2023-06-16 00:11:14)
 이미 사용하고 있는 구분자
@@ -230,12 +383,35 @@
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
 v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="C4">
+  </commentList>
+  <extLst>
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mg9x9zo1dI2zhea+x/YhgCiYCYGtw=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbSc
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbSQ
 UISU    (2023-06-16 00:11:14)
 0: NONE
 1: 대화
@@ -250,24 +426,20 @@
 6: CutScene
 7: WaitInteract
 8: Interact</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="E4">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbR0
-UISU    (2023-06-16 00:11:14)
-Default = -1
-Keep = 0 (이전 유지), (기본)
-Action1 = 1
-…
-Option에서 Left or Right 필수</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D4">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRY
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbSM
 UISU    (2023-06-16 00:11:14)
 Dubby = -1,
     Keep = 0,
@@ -279,26 +451,19 @@
     Dog = 6,
     PhotographerSon = 7,
     PhotographerWife = 8,</t>
+        </r>
       </text>
     </comment>
-  </commentList>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mg9x9zo1dI2zhea+x/YhgCiYCYGtw=="/>
-    </ext>
-  </extLst>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="E4">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbS0
 UISU    (2023-06-16 00:11:14)
 Default = -1
@@ -306,11 +471,19 @@
 Action1 = 1
 …
 Option에서 Left or Right 필수</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="F4">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSw
 서 의수    (2023-06-16 00:11:14)
 이미 사용하고 있는 구분자
@@ -332,12 +505,35 @@
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
 v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="C4">
+  </commentList>
+  <extLst>
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miS7bgLk+Wj2R3Tr0V8rO7GVbQoCg=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbSQ
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRw
 UISU    (2023-06-16 00:11:14)
 0: NONE
 1: 대화
@@ -352,12 +548,20 @@
 6: CutScene
 7: WaitInteract
 8: Interact</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="D4">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbSM
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbR4
 UISU    (2023-06-16 00:11:14)
 Dubby = -1,
     Keep = 0,
@@ -369,26 +573,19 @@
     Dog = 6,
     PhotographerSon = 7,
     PhotographerWife = 8,</t>
+        </r>
       </text>
     </comment>
-  </commentList>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miS7bgLk+Wj2R3Tr0V8rO7GVbQoCg=="/>
-    </ext>
-  </extLst>
-</comments>
-</file>
-
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="E4">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSo
 UISU    (2023-06-16 00:11:14)
 Default = -1
@@ -396,11 +593,19 @@
 Action1 = 1
 …
 Option에서 Left or Right 필수</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="F4">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSI
 서 의수    (2023-06-16 00:11:14)
 이미 사용하고 있는 구분자
@@ -422,48 +627,12 @@
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
 v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D4">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbR4
-UISU    (2023-06-16 00:11:14)
-Dubby = -1,
-    Keep = 0,
-    None = 1,
-    Protagonist = 2,
-    Naru = 3,
-    Photographer = 4,
-    Doctor = 5,
-    Dog = 6,
-    PhotographerSon = 7,
-    PhotographerWife = 8,</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="C4">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRw
-UISU    (2023-06-16 00:11:14)
-0: NONE
-1: 대화
-2: 선택지 (1, 2, 3)
-3: 선택지 종료
-4: 맵 이동 (이동할 Scene 이름 - contents)
-5: Save
-9: Random
-10: Random End
-11: Immediately Execute
-// Inspector창에서 직접 조정
-6: CutScene
-7: WaitInteract
-8: Interact</t>
+        </r>
       </text>
     </comment>
   </commentList>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mj7dVX2vI5HqNPSBDYbuJcE0aPrxA=="/>
     </ext>
   </extLst>
@@ -471,14 +640,21 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C4">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSE
 UISU    (2023-06-16 00:11:14)
 0: NONE
@@ -494,11 +670,64 @@
 6: CutScene
 7: WaitInteract
 8: Interact</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="F4">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRo
+UISU    (2023-06-16 00:11:14)
+Dubby = -1,
+    Keep = 0,
+    None = 1,
+    Protagonist = 2,
+    Naru = 3,
+    Photographer = 4,
+    Doctor = 5,
+    Dog = 6,
+    PhotographerSon = 7,
+    PhotographerWife = 8,</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRs
+UISU    (2023-06-16 00:11:14)
+Default = -1
+Keep = 0 (이전 유지), (기본)
+Action1 = 1
+…
+Option에서 Left or Right 필수</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbR8
 서 의수    (2023-06-16 00:11:14)
 이미 사용하고 있는 구분자
@@ -520,40 +749,12 @@
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
 v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="E4">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRs
-UISU    (2023-06-16 00:11:14)
-Default = -1
-Keep = 0 (이전 유지), (기본)
-Action1 = 1
-…
-Option에서 Left or Right 필수</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D4">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRo
-UISU    (2023-06-16 00:11:14)
-Dubby = -1,
-    Keep = 0,
-    None = 1,
-    Protagonist = 2,
-    Naru = 3,
-    Photographer = 4,
-    Doctor = 5,
-    Dog = 6,
-    PhotographerSon = 7,
-    PhotographerWife = 8,</t>
+        </r>
       </text>
     </comment>
   </commentList>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhYtCu5D0iitr1q5hlRkR58d3RMfw=="/>
     </ext>
   </extLst>
@@ -748,9 +949,6 @@
     <t>(머리를 쓰다듬는다.)</t>
   </si>
   <si>
-    <t>2,0,1,0</t>
-  </si>
-  <si>
     <t>&lt;시스템&gt;</t>
   </si>
   <si>
@@ -758,9 +956,6 @@
   </si>
   <si>
     <t>(발로 찬다.)</t>
-  </si>
-  <si>
-    <t>2,0,2,0</t>
   </si>
   <si>
     <t>열쇠 &lt;b&gt;&lt;극단&gt;&lt;/b&gt;을 획득하였다.</t>
@@ -819,32 +1014,52 @@
   <si>
     <t>···운행하고 있는 건가?</t>
   </si>
+  <si>
+    <t>Tendency-감내</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tendency-극단</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="A고딕12"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -852,7 +1067,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -874,7 +1089,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -888,85 +1109,65 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1156,29 +1357,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.86"/>
+    <col min="1" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="16.5" customHeight="1">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1198,7 +1401,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1218,7 +1421,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1238,18 +1441,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="16.5" customHeight="1"/>
-    <row r="6" ht="16.5" customHeight="1"/>
-    <row r="7" ht="16.5" customHeight="1"/>
-    <row r="8" ht="16.5" customHeight="1"/>
-    <row r="9" ht="16.5" customHeight="1"/>
-    <row r="10" ht="16.5" customHeight="1"/>
-    <row r="11" ht="16.5" customHeight="1"/>
-    <row r="12" ht="16.5" customHeight="1"/>
-    <row r="13" ht="16.5" customHeight="1"/>
-    <row r="14" ht="16.5" customHeight="1"/>
-    <row r="15" ht="16.5" customHeight="1"/>
-    <row r="16" ht="16.5" customHeight="1"/>
+    <row r="5" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="6" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="7" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="8" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="11" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="15" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="17" ht="16.5" customHeight="1"/>
     <row r="18" ht="16.5" customHeight="1"/>
     <row r="19" ht="16.5" customHeight="1"/>
@@ -2235,39 +2438,36 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.86"/>
-    <col customWidth="1" min="2" max="2" width="89.0"/>
-    <col customWidth="1" min="3" max="4" width="25.0"/>
-    <col customWidth="1" min="5" max="5" width="21.43"/>
-    <col customWidth="1" min="6" max="6" width="9.57"/>
-    <col customWidth="1" min="7" max="26" width="8.86"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="89" customWidth="1"/>
+    <col min="3" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
+    <row r="1" spans="1:16" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" ht="16.5" customHeight="1">
+    <row r="2" spans="1:16" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2287,7 +2487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1">
+    <row r="3" spans="1:16" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2307,7 +2507,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:16" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2327,7 +2527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="16.5" customHeight="1">
+    <row r="5" spans="1:16" ht="16.5" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -2335,17 +2535,17 @@
         <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" ht="16.5" customHeight="1">
+    <row r="6" spans="1:16" ht="16.5" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -2353,31 +2553,31 @@
         <v>22</v>
       </c>
       <c r="C6" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" ht="16.5" customHeight="1">
+    <row r="7" spans="1:16" ht="16.5" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" ht="16.5" customHeight="1">
+    <row r="8" spans="1:16" ht="16.5" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -2385,17 +2585,17 @@
         <v>27</v>
       </c>
       <c r="C8" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" ht="16.5" customHeight="1">
+    <row r="9" spans="1:16" ht="16.5" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -2403,15 +2603,15 @@
         <v>29</v>
       </c>
       <c r="C9" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" ht="16.5" customHeight="1">
+    <row r="10" spans="1:16" ht="16.5" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -2419,27 +2619,27 @@
         <v>30</v>
       </c>
       <c r="C10" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" ht="16.5" customHeight="1">
+    <row r="11" spans="1:16" ht="16.5" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" ht="16.5" customHeight="1">
+    <row r="12" spans="1:16" ht="16.5" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -2447,17 +2647,17 @@
         <v>32</v>
       </c>
       <c r="C12" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" ht="16.5" customHeight="1">
+    <row r="13" spans="1:16" ht="16.5" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
@@ -2465,17 +2665,17 @@
         <v>32</v>
       </c>
       <c r="C13" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" ht="16.5" customHeight="1">
+    <row r="14" spans="1:16" ht="16.5" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -2483,19 +2683,19 @@
         <v>33</v>
       </c>
       <c r="C14" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" ht="16.5" customHeight="1">
+    <row r="15" spans="1:16" ht="16.5" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2503,233 +2703,233 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" ht="16.5" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7" t="s">
+    <row r="16" spans="1:16" ht="16.5" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" ht="16.5" customHeight="1">
-      <c r="A17" s="6" t="s">
+      <c r="C16" s="5">
+        <v>7</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D17" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6" t="s">
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
+        <v>4</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" ht="16.5" customHeight="1">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6">
-        <v>11.0</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6" t="s">
+    <row r="18" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5">
+        <v>11</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" ht="16.5" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7" t="s">
+    <row r="19" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" ht="16.5" customHeight="1"/>
-    <row r="21" ht="16.5" customHeight="1"/>
-    <row r="22" ht="16.5" customHeight="1">
-      <c r="B22" s="8"/>
-    </row>
-    <row r="23" ht="16.5" customHeight="1">
-      <c r="B23" s="8"/>
-    </row>
-    <row r="24" ht="16.5" customHeight="1">
-      <c r="B24" s="8"/>
-    </row>
-    <row r="25" ht="16.5" customHeight="1">
-      <c r="B25" s="8"/>
-    </row>
-    <row r="26" ht="16.5" customHeight="1">
-      <c r="B26" s="8"/>
-    </row>
-    <row r="27" ht="16.5" customHeight="1">
-      <c r="B27" s="8"/>
-    </row>
-    <row r="28" ht="16.5" customHeight="1">
-      <c r="B28" s="8"/>
-    </row>
-    <row r="29" ht="16.5" customHeight="1">
-      <c r="B29" s="8"/>
-    </row>
-    <row r="30" ht="16.5" customHeight="1"/>
-    <row r="31" ht="16.5" customHeight="1"/>
-    <row r="32" ht="16.5" customHeight="1">
-      <c r="B32" s="8"/>
-    </row>
-    <row r="33" ht="16.5" customHeight="1"/>
-    <row r="34" ht="16.5" customHeight="1"/>
-    <row r="35" ht="16.5" customHeight="1"/>
-    <row r="36" ht="16.5" customHeight="1"/>
-    <row r="37" ht="16.5" customHeight="1"/>
-    <row r="38" ht="16.5" customHeight="1"/>
-    <row r="39" ht="16.5" customHeight="1"/>
-    <row r="40" ht="16.5" customHeight="1"/>
-    <row r="41" ht="16.5" customHeight="1"/>
-    <row r="42" ht="16.5" customHeight="1"/>
-    <row r="43" ht="16.5" customHeight="1"/>
-    <row r="44" ht="16.5" customHeight="1"/>
-    <row r="45" ht="16.5" customHeight="1"/>
-    <row r="46" ht="16.5" customHeight="1"/>
-    <row r="47" ht="16.5" customHeight="1">
-      <c r="A47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="8"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="8"/>
-      <c r="Q47" s="8"/>
-      <c r="R47" s="8"/>
-      <c r="S47" s="8"/>
-      <c r="T47" s="8"/>
-      <c r="U47" s="8"/>
-      <c r="V47" s="8"/>
-      <c r="W47" s="8"/>
-      <c r="X47" s="8"/>
-      <c r="Y47" s="8"/>
-      <c r="Z47" s="8"/>
-    </row>
-    <row r="48" ht="16.5" customHeight="1">
-      <c r="A48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
-      <c r="R48" s="8"/>
-      <c r="S48" s="8"/>
-      <c r="T48" s="8"/>
-      <c r="U48" s="8"/>
-      <c r="V48" s="8"/>
-      <c r="W48" s="8"/>
-      <c r="X48" s="8"/>
-      <c r="Y48" s="8"/>
-      <c r="Z48" s="8"/>
-    </row>
-    <row r="49" ht="16.5" customHeight="1">
-      <c r="B49" s="8"/>
-    </row>
-    <row r="50" ht="16.5" customHeight="1">
-      <c r="B50" s="8"/>
-    </row>
-    <row r="51" ht="16.5" customHeight="1">
-      <c r="B51" s="8"/>
-    </row>
-    <row r="52" ht="16.5" customHeight="1">
-      <c r="B52" s="8"/>
-    </row>
-    <row r="53" ht="16.5" customHeight="1">
-      <c r="B53" s="8"/>
-    </row>
-    <row r="54" ht="16.5" customHeight="1">
-      <c r="B54" s="8"/>
-    </row>
-    <row r="55" ht="16.5" customHeight="1">
-      <c r="B55" s="8"/>
-    </row>
-    <row r="56" ht="16.5" customHeight="1">
-      <c r="B56" s="8"/>
-    </row>
-    <row r="57" ht="16.5" customHeight="1">
-      <c r="B57" s="8"/>
-    </row>
-    <row r="58" ht="16.5" customHeight="1">
-      <c r="B58" s="8"/>
-    </row>
-    <row r="59" ht="16.5" customHeight="1">
-      <c r="B59" s="8"/>
-    </row>
-    <row r="60" ht="16.5" customHeight="1">
-      <c r="B60" s="8"/>
-    </row>
-    <row r="61" ht="16.5" customHeight="1">
-      <c r="B61" s="8"/>
-    </row>
-    <row r="62" ht="16.5" customHeight="1">
-      <c r="B62" s="8"/>
-    </row>
-    <row r="63" ht="16.5" customHeight="1">
-      <c r="B63" s="8"/>
-    </row>
-    <row r="64" ht="16.5" customHeight="1"/>
-    <row r="65" ht="16.5" customHeight="1"/>
-    <row r="66" ht="16.5" customHeight="1">
-      <c r="B66" s="8"/>
-    </row>
-    <row r="67" ht="16.5" customHeight="1">
-      <c r="B67" s="8"/>
-    </row>
-    <row r="68" ht="16.5" customHeight="1">
-      <c r="B68" s="8"/>
-    </row>
-    <row r="69" ht="16.5" customHeight="1"/>
-    <row r="70" ht="16.5" customHeight="1"/>
-    <row r="71" ht="16.5" customHeight="1">
-      <c r="B71" s="8"/>
-    </row>
-    <row r="72" ht="16.5" customHeight="1">
-      <c r="B72" s="8"/>
-    </row>
-    <row r="73" ht="16.5" customHeight="1">
-      <c r="B73" s="8"/>
-    </row>
-    <row r="74" ht="16.5" customHeight="1"/>
-    <row r="75" ht="16.5" customHeight="1"/>
-    <row r="76" ht="16.5" customHeight="1"/>
-    <row r="77" ht="16.5" customHeight="1"/>
-    <row r="78" ht="16.5" customHeight="1"/>
-    <row r="79" ht="16.5" customHeight="1"/>
-    <row r="80" ht="16.5" customHeight="1"/>
+      <c r="C19" s="5">
+        <v>7</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="21" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="22" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="31" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="32" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="34" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="35" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="36" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="37" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="38" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="39" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="40" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="41" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="42" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="43" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="44" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="45" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="46" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="47" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
+      <c r="S47" s="7"/>
+      <c r="T47" s="7"/>
+      <c r="U47" s="7"/>
+      <c r="V47" s="7"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="7"/>
+      <c r="Y47" s="7"/>
+      <c r="Z47" s="7"/>
+    </row>
+    <row r="48" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
+      <c r="S48" s="7"/>
+      <c r="T48" s="7"/>
+      <c r="U48" s="7"/>
+      <c r="V48" s="7"/>
+      <c r="W48" s="7"/>
+      <c r="X48" s="7"/>
+      <c r="Y48" s="7"/>
+      <c r="Z48" s="7"/>
+    </row>
+    <row r="49" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B49" s="7"/>
+    </row>
+    <row r="50" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B50" s="7"/>
+    </row>
+    <row r="51" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B51" s="7"/>
+    </row>
+    <row r="52" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B52" s="7"/>
+    </row>
+    <row r="53" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B53" s="7"/>
+    </row>
+    <row r="54" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B54" s="7"/>
+    </row>
+    <row r="55" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B55" s="7"/>
+    </row>
+    <row r="56" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B56" s="7"/>
+    </row>
+    <row r="57" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B57" s="7"/>
+    </row>
+    <row r="58" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B58" s="7"/>
+    </row>
+    <row r="59" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B59" s="7"/>
+    </row>
+    <row r="60" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B60" s="7"/>
+    </row>
+    <row r="61" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B61" s="7"/>
+    </row>
+    <row r="62" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B62" s="7"/>
+    </row>
+    <row r="63" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B63" s="7"/>
+    </row>
+    <row r="64" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="65" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="66" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B66" s="7"/>
+    </row>
+    <row r="67" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B67" s="7"/>
+    </row>
+    <row r="68" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B68" s="7"/>
+    </row>
+    <row r="69" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="70" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="71" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B71" s="7"/>
+    </row>
+    <row r="72" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B72" s="7"/>
+    </row>
+    <row r="73" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B73" s="7"/>
+    </row>
+    <row r="74" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="75" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="76" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="77" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="78" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="79" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="80" spans="2:2" ht="16.5" customHeight="1"/>
     <row r="81" ht="16.5" customHeight="1"/>
     <row r="82" ht="16.5" customHeight="1"/>
     <row r="83" ht="16.5" customHeight="1"/>
@@ -3651,39 +3851,38 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="11.0"/>
-    <col customWidth="1" min="2" max="2" width="70.43"/>
-    <col customWidth="1" min="3" max="3" width="16.14"/>
-    <col customWidth="1" min="4" max="4" width="18.14"/>
-    <col customWidth="1" min="5" max="5" width="15.43"/>
-    <col customWidth="1" min="6" max="6" width="51.43"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="70.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" ht="16.5" customHeight="1">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3703,7 +3902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -3723,7 +3922,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -3743,442 +3942,442 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="16.5" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9" t="s">
+      <c r="C5" s="8">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" ht="16.5" customHeight="1">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9" t="s">
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" ht="16.5" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A7" s="10"/>
+      <c r="B7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9" t="s">
+      <c r="C7" s="8">
+        <v>6</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" ht="16.5" customHeight="1">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" ht="16.5" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9" t="s">
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9" t="s">
+      <c r="C9" s="8">
+        <v>6</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" ht="16.5" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9">
-        <v>11.0</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9" t="s">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8">
+        <v>11</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" ht="16.5" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9" t="s">
+      <c r="C11" s="8">
+        <v>6</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" ht="16.5" customHeight="1">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" ht="16.5" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="C12" s="8">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A13" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" ht="16.5" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10" t="s">
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9" t="s">
+      <c r="C14" s="8">
+        <v>6</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" ht="16.5" customHeight="1">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" ht="16.5" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10" t="s">
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9" t="s">
+      <c r="C16" s="8">
+        <v>6</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" ht="16.5" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10" t="s">
+    <row r="17" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9" t="s">
+      <c r="C17" s="8">
+        <v>6</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" ht="16.5" customHeight="1">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A18" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D18" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9" t="s">
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8">
+        <v>6</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" ht="16.5" customHeight="1">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D19" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9" t="s">
+      <c r="C19" s="8">
+        <v>1</v>
+      </c>
+      <c r="D19" s="8">
+        <v>4</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" ht="16.5" customHeight="1">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D20" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" ht="16.5" customHeight="1">
-      <c r="A21" s="9" t="s">
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8">
+        <v>6</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D21" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" ht="16.5" customHeight="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10" t="s">
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+      <c r="D21" s="8">
+        <v>4</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9" t="s">
+      <c r="C22" s="8">
+        <v>2</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A23" s="8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" ht="16.5" customHeight="1">
-      <c r="A23" s="9" t="s">
+      <c r="B23" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="C23" s="8">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-    </row>
-    <row r="24" ht="16.5" customHeight="1">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="8">
+        <v>2</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A25" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9" t="s">
+      <c r="C25" s="8">
+        <v>1</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="8">
+        <v>3</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A27" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A28" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" ht="16.5" customHeight="1">
-      <c r="A25" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="10" t="s">
+      <c r="C28" s="8">
+        <v>1</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A29" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" ht="16.5" customHeight="1">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="9">
-        <v>3.0</v>
-      </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" ht="16.5" customHeight="1">
-      <c r="A27" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" ht="16.5" customHeight="1">
-      <c r="A28" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="10" t="s">
+      <c r="C29" s="8">
+        <v>1</v>
+      </c>
+      <c r="D29" s="8">
+        <v>6</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8">
+        <v>11</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-    </row>
-    <row r="29" ht="16.5" customHeight="1">
-      <c r="A29" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="9" t="s">
+      <c r="C31" s="8">
+        <v>7</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D29" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" ht="16.5" customHeight="1">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9">
-        <v>11.0</v>
-      </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" ht="16.5" customHeight="1">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9" t="s">
+      <c r="C32" s="8">
+        <v>11</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8">
+        <v>5</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="9">
-        <v>7.0</v>
-      </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32" ht="16.5" customHeight="1">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="9">
-        <v>11.0</v>
-      </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" ht="16.5" customHeight="1">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9">
-        <v>5.0</v>
-      </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" ht="16.5" customHeight="1">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" ht="16.5" customHeight="1"/>
-    <row r="36" ht="16.5" customHeight="1"/>
-    <row r="37" ht="16.5" customHeight="1"/>
-    <row r="38" ht="16.5" customHeight="1"/>
-    <row r="39" ht="16.5" customHeight="1"/>
-    <row r="40" ht="16.5" customHeight="1"/>
-    <row r="41" ht="16.5" customHeight="1"/>
-    <row r="42" ht="16.5" customHeight="1"/>
-    <row r="43" ht="16.5" customHeight="1"/>
-    <row r="44" ht="16.5" customHeight="1"/>
-    <row r="45" ht="16.5" customHeight="1"/>
-    <row r="46" ht="16.5" customHeight="1"/>
-    <row r="47" ht="16.5" customHeight="1"/>
-    <row r="48" ht="16.5" customHeight="1"/>
+      <c r="C34" s="8">
+        <v>4</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="36" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="37" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="38" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="39" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="40" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="41" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="42" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="43" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="44" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="45" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="46" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="47" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="48" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="49" ht="16.5" customHeight="1"/>
     <row r="50" ht="16.5" customHeight="1"/>
     <row r="51" ht="16.5" customHeight="1"/>
@@ -5132,38 +5331,35 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.43"/>
-    <col customWidth="1" min="2" max="2" width="59.14"/>
-    <col customWidth="1" min="3" max="4" width="25.0"/>
-    <col customWidth="1" min="5" max="5" width="21.43"/>
-    <col customWidth="1" min="6" max="6" width="9.57"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" customWidth="1"/>
+    <col min="3" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" ht="16.5" customHeight="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -5183,7 +5379,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -5203,7 +5399,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -5223,80 +5419,80 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="16.5" customHeight="1">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" ht="16.5" customHeight="1">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" ht="16.5" customHeight="1">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="8" ht="16.5" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C8" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9" ht="16.5" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="C9" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" ht="16.5" customHeight="1"/>
-    <row r="11" ht="16.5" customHeight="1"/>
-    <row r="12" ht="16.5" customHeight="1"/>
-    <row r="13" ht="16.5" customHeight="1"/>
-    <row r="14" ht="16.5" customHeight="1"/>
-    <row r="15" ht="16.5" customHeight="1"/>
-    <row r="16" ht="16.5" customHeight="1"/>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="11" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="15" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="17" ht="16.5" customHeight="1"/>
     <row r="18" ht="16.5" customHeight="1"/>
     <row r="19" ht="16.5" customHeight="1"/>
@@ -6282,43 +6478,40 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.43"/>
-    <col customWidth="1" min="2" max="2" width="29.14"/>
-    <col customWidth="1" min="3" max="4" width="25.0"/>
-    <col customWidth="1" min="5" max="5" width="21.43"/>
-    <col customWidth="1" min="6" max="6" width="9.57"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
-      <c r="A1" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" ht="16.5" customHeight="1">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6338,7 +6531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -6358,7 +6551,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -6378,55 +6571,55 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="16.5" customHeight="1">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" ht="16.5" customHeight="1">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" ht="16.5" customHeight="1">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="8" ht="16.5" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -6434,13 +6627,13 @@
         <v>32</v>
       </c>
       <c r="C8" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="9" ht="16.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -6448,36 +6641,36 @@
         <v>32</v>
       </c>
       <c r="C9" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="10" ht="16.5" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C10" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="11" ht="16.5" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="C11" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" ht="16.5" customHeight="1"/>
-    <row r="13" ht="16.5" customHeight="1"/>
-    <row r="14" ht="16.5" customHeight="1"/>
-    <row r="15" ht="16.5" customHeight="1"/>
-    <row r="16" ht="16.5" customHeight="1"/>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="15" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="17" ht="16.5" customHeight="1"/>
     <row r="18" ht="16.5" customHeight="1"/>
     <row r="19" ht="16.5" customHeight="1"/>
@@ -7463,43 +7656,40 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.43"/>
-    <col customWidth="1" min="2" max="2" width="24.43"/>
-    <col customWidth="1" min="3" max="4" width="25.0"/>
-    <col customWidth="1" min="5" max="5" width="21.43"/>
-    <col customWidth="1" min="6" max="6" width="9.57"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
-      <c r="A1" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" ht="16.5" customHeight="1">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7519,7 +7709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -7539,7 +7729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -7559,51 +7749,51 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="16.5" customHeight="1">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" ht="16.5" customHeight="1">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C6" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7" ht="16.5" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" customHeight="1">
       <c r="C7" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" ht="16.5" customHeight="1"/>
-    <row r="9" ht="16.5" customHeight="1"/>
-    <row r="10" ht="16.5" customHeight="1"/>
-    <row r="11" ht="16.5" customHeight="1"/>
-    <row r="12" ht="16.5" customHeight="1"/>
-    <row r="13" ht="16.5" customHeight="1"/>
-    <row r="14" ht="16.5" customHeight="1"/>
-    <row r="15" ht="16.5" customHeight="1"/>
-    <row r="16" ht="16.5" customHeight="1"/>
+    <row r="8" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="11" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="15" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="17" ht="16.5" customHeight="1"/>
     <row r="18" ht="16.5" customHeight="1"/>
     <row r="19" ht="16.5" customHeight="1"/>
@@ -8589,10 +8779,9 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update UI & Necklace Tendency word UI (#99)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage1/Beach.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage1/Beach.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B9BB5D-75F2-44FF-8E83-815B3018BBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="!Sample" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="1-3 main-0" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="1-3 main-1" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="1-3, 1" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="1-3, 2" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="1-3, 3" sheetId="6" r:id="rId9"/>
+    <sheet name="!Sample" sheetId="1" r:id="rId1"/>
+    <sheet name="1-3 main-0" sheetId="2" r:id="rId2"/>
+    <sheet name="1-3 main-1" sheetId="3" r:id="rId3"/>
+    <sheet name="1-3, 1" sheetId="4" r:id="rId4"/>
+    <sheet name="1-3, 2" sheetId="5" r:id="rId5"/>
+    <sheet name="1-3, 3" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="z+DT7o7porseD4XXZZXxVcYexPRtbcPrOX3Ci11Z6AE="/>
@@ -21,14 +30,74 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="E4">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRk
+UISU    (2023-06-16 00:11:14)
+0: NONE
+1: 대화
+2: 선택지 (1, 2, 3)
+3: 선택지 종료
+4: 맵 이동 (이동할 Scene 이름 - contents)
+5: Save
+9: Random
+10: Random End
+11: Immediately Execute
+// Inspector창에서 직접 조정
+6: CutScene
+7: WaitInteract
+8: Interact</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRc
+UISU    (2023-06-16 00:11:14)
+Dubby = -1,
+    Keep = 0,
+    None = 1,
+    Protagonist = 2,
+    Naru = 3,
+    Photographer = 4,
+    Doctor = 5,
+    Dog = 6,
+    PhotographerSon = 7,
+    PhotographerWife = 8,</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSU
 UISU    (2023-06-16 00:11:14)
 Default = -1
@@ -36,11 +105,19 @@
 Action1 = 1
 …
 Option에서 Left or Right 필수</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="F4">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSA
 서 의수    (2023-06-16 00:11:14)
 이미 사용하고 있는 구분자
@@ -62,12 +139,35 @@
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
 v2 - true, false 다음 Index로 Auto 여부 (Default - true)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="C4">
+  </commentList>
+  <extLst>
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjK335ix46titMzMPgIl0zgeEef9Q=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRk
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRg
 UISU    (2023-06-16 00:11:14)
 0: NONE
 1: 대화
@@ -82,43 +182,19 @@
 6: CutScene
 7: WaitInteract
 8: Interact</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="D4">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRc
-UISU    (2023-06-16 00:11:14)
-Dubby = -1,
-    Keep = 0,
-    None = 1,
-    Protagonist = 2,
-    Naru = 3,
-    Photographer = 4,
-    Doctor = 5,
-    Dog = 6,
-    PhotographerSon = 7,
-    PhotographerWife = 8,</t>
-      </text>
-    </comment>
-  </commentList>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjK335ix46titMzMPgIl0zgeEef9Q=="/>
-    </ext>
-  </extLst>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="D4">
-      <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSs
 UISU    (2023-06-16 00:11:14)
 Dubby = -1,
@@ -131,11 +207,39 @@
     Dog = 6,
     PhotographerSon = 7,
     PhotographerWife = 8,</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="F4">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbSY
+UISU    (2023-06-16 00:11:14)
+Default = -1
+Keep = 0 (이전 유지), (기본)
+Action1 = 1
+…
+Option에서 Left or Right 필수</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSk
 서 의수    (2023-06-16 00:11:14)
 이미 사용하고 있는 구분자
@@ -157,24 +261,35 @@
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
 v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="E4">
+  </commentList>
+  <extLst>
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgJDK4yi5U9B8/yWEBOphYrXagDfQ=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbSY
-UISU    (2023-06-16 00:11:14)
-Default = -1
-Keep = 0 (이전 유지), (기본)
-Action1 = 1
-…
-Option에서 Left or Right 필수</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="C4">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRg
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbSc
 UISU    (2023-06-16 00:11:14)
 0: NONE
 1: 대화
@@ -189,26 +304,64 @@
 6: CutScene
 7: WaitInteract
 8: Interact</t>
+        </r>
       </text>
     </comment>
-  </commentList>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgJDK4yi5U9B8/yWEBOphYrXagDfQ=="/>
-    </ext>
-  </extLst>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="F4">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRY
+UISU    (2023-06-16 00:11:14)
+Dubby = -1,
+    Keep = 0,
+    None = 1,
+    Protagonist = 2,
+    Naru = 3,
+    Photographer = 4,
+    Doctor = 5,
+    Dog = 6,
+    PhotographerSon = 7,
+    PhotographerWife = 8,</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbR0
+UISU    (2023-06-16 00:11:14)
+Default = -1
+Keep = 0 (이전 유지), (기본)
+Action1 = 1
+…
+Option에서 Left or Right 필수</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSg
 서 의수    (2023-06-16 00:11:14)
 이미 사용하고 있는 구분자
@@ -230,12 +383,35 @@
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
 v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="C4">
+  </commentList>
+  <extLst>
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mg9x9zo1dI2zhea+x/YhgCiYCYGtw=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbSc
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbSQ
 UISU    (2023-06-16 00:11:14)
 0: NONE
 1: 대화
@@ -250,24 +426,20 @@
 6: CutScene
 7: WaitInteract
 8: Interact</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="E4">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbR0
-UISU    (2023-06-16 00:11:14)
-Default = -1
-Keep = 0 (이전 유지), (기본)
-Action1 = 1
-…
-Option에서 Left or Right 필수</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D4">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRY
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbSM
 UISU    (2023-06-16 00:11:14)
 Dubby = -1,
     Keep = 0,
@@ -279,26 +451,19 @@
     Dog = 6,
     PhotographerSon = 7,
     PhotographerWife = 8,</t>
+        </r>
       </text>
     </comment>
-  </commentList>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mg9x9zo1dI2zhea+x/YhgCiYCYGtw=="/>
-    </ext>
-  </extLst>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="E4">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbS0
 UISU    (2023-06-16 00:11:14)
 Default = -1
@@ -306,11 +471,19 @@
 Action1 = 1
 …
 Option에서 Left or Right 필수</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="F4">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSw
 서 의수    (2023-06-16 00:11:14)
 이미 사용하고 있는 구분자
@@ -332,12 +505,35 @@
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
 v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="C4">
+  </commentList>
+  <extLst>
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miS7bgLk+Wj2R3Tr0V8rO7GVbQoCg=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbSQ
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRw
 UISU    (2023-06-16 00:11:14)
 0: NONE
 1: 대화
@@ -352,12 +548,20 @@
 6: CutScene
 7: WaitInteract
 8: Interact</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="D4">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbSM
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbR4
 UISU    (2023-06-16 00:11:14)
 Dubby = -1,
     Keep = 0,
@@ -369,26 +573,19 @@
     Dog = 6,
     PhotographerSon = 7,
     PhotographerWife = 8,</t>
+        </r>
       </text>
     </comment>
-  </commentList>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miS7bgLk+Wj2R3Tr0V8rO7GVbQoCg=="/>
-    </ext>
-  </extLst>
-</comments>
-</file>
-
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="E4">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSo
 UISU    (2023-06-16 00:11:14)
 Default = -1
@@ -396,11 +593,19 @@
 Action1 = 1
 …
 Option에서 Left or Right 필수</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="F4">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSI
 서 의수    (2023-06-16 00:11:14)
 이미 사용하고 있는 구분자
@@ -422,48 +627,12 @@
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
 v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D4">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbR4
-UISU    (2023-06-16 00:11:14)
-Dubby = -1,
-    Keep = 0,
-    None = 1,
-    Protagonist = 2,
-    Naru = 3,
-    Photographer = 4,
-    Doctor = 5,
-    Dog = 6,
-    PhotographerSon = 7,
-    PhotographerWife = 8,</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="C4">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRw
-UISU    (2023-06-16 00:11:14)
-0: NONE
-1: 대화
-2: 선택지 (1, 2, 3)
-3: 선택지 종료
-4: 맵 이동 (이동할 Scene 이름 - contents)
-5: Save
-9: Random
-10: Random End
-11: Immediately Execute
-// Inspector창에서 직접 조정
-6: CutScene
-7: WaitInteract
-8: Interact</t>
+        </r>
       </text>
     </comment>
   </commentList>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mj7dVX2vI5HqNPSBDYbuJcE0aPrxA=="/>
     </ext>
   </extLst>
@@ -471,14 +640,21 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C4">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbSE
 UISU    (2023-06-16 00:11:14)
 0: NONE
@@ -494,11 +670,64 @@
 6: CutScene
 7: WaitInteract
 8: Interact</t>
+        </r>
       </text>
     </comment>
-    <comment authorId="0" ref="F4">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
-        <t xml:space="preserve">======
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRo
+UISU    (2023-06-16 00:11:14)
+Dubby = -1,
+    Keep = 0,
+    None = 1,
+    Protagonist = 2,
+    Naru = 3,
+    Photographer = 4,
+    Doctor = 5,
+    Dog = 6,
+    PhotographerSon = 7,
+    PhotographerWife = 8,</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAAAzYERbRs
+UISU    (2023-06-16 00:11:14)
+Default = -1
+Keep = 0 (이전 유지), (기본)
+Action1 = 1
+…
+Option에서 Left or Right 필수</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
 ID#AAAAzYERbR8
 서 의수    (2023-06-16 00:11:14)
 이미 사용하고 있는 구분자
@@ -520,40 +749,12 @@
 v1 - value : {$value}초 이후 스킵이 가능해진다. 없으면 0초 후 가능(number)
 v2 - true, false 다음 Index로 Auto 여부 (Default - false)  (대소문자 무관)
 v3 - name=value (Resources/Timeline/{$value}) 폴더에서 불러옴, 없으면 직접 넣는다. (string)</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="E4">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRs
-UISU    (2023-06-16 00:11:14)
-Default = -1
-Keep = 0 (이전 유지), (기본)
-Action1 = 1
-…
-Option에서 Left or Right 필수</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D4">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAzYERbRo
-UISU    (2023-06-16 00:11:14)
-Dubby = -1,
-    Keep = 0,
-    None = 1,
-    Protagonist = 2,
-    Naru = 3,
-    Photographer = 4,
-    Doctor = 5,
-    Dog = 6,
-    PhotographerSon = 7,
-    PhotographerWife = 8,</t>
+        </r>
       </text>
     </comment>
   </commentList>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
+    <ext xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhYtCu5D0iitr1q5hlRkR58d3RMfw=="/>
     </ext>
   </extLst>
@@ -748,9 +949,6 @@
     <t>(머리를 쓰다듬는다.)</t>
   </si>
   <si>
-    <t>2,0,1,0</t>
-  </si>
-  <si>
     <t>&lt;시스템&gt;</t>
   </si>
   <si>
@@ -758,9 +956,6 @@
   </si>
   <si>
     <t>(발로 찬다.)</t>
-  </si>
-  <si>
-    <t>2,0,2,0</t>
   </si>
   <si>
     <t>열쇠 &lt;b&gt;&lt;극단&gt;&lt;/b&gt;을 획득하였다.</t>
@@ -819,32 +1014,52 @@
   <si>
     <t>···운행하고 있는 건가?</t>
   </si>
+  <si>
+    <t>Tendency-감내</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tendency-극단</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="A고딕12"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -852,7 +1067,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -874,7 +1089,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -888,85 +1109,65 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1156,29 +1357,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.86"/>
+    <col min="1" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="16.5" customHeight="1">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1198,7 +1401,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1218,7 +1421,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1238,18 +1441,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="16.5" customHeight="1"/>
-    <row r="6" ht="16.5" customHeight="1"/>
-    <row r="7" ht="16.5" customHeight="1"/>
-    <row r="8" ht="16.5" customHeight="1"/>
-    <row r="9" ht="16.5" customHeight="1"/>
-    <row r="10" ht="16.5" customHeight="1"/>
-    <row r="11" ht="16.5" customHeight="1"/>
-    <row r="12" ht="16.5" customHeight="1"/>
-    <row r="13" ht="16.5" customHeight="1"/>
-    <row r="14" ht="16.5" customHeight="1"/>
-    <row r="15" ht="16.5" customHeight="1"/>
-    <row r="16" ht="16.5" customHeight="1"/>
+    <row r="5" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="6" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="7" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="8" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="11" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="15" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="17" ht="16.5" customHeight="1"/>
     <row r="18" ht="16.5" customHeight="1"/>
     <row r="19" ht="16.5" customHeight="1"/>
@@ -2235,39 +2438,36 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.86"/>
-    <col customWidth="1" min="2" max="2" width="89.0"/>
-    <col customWidth="1" min="3" max="4" width="25.0"/>
-    <col customWidth="1" min="5" max="5" width="21.43"/>
-    <col customWidth="1" min="6" max="6" width="9.57"/>
-    <col customWidth="1" min="7" max="26" width="8.86"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="89" customWidth="1"/>
+    <col min="3" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
+    <row r="1" spans="1:16" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" ht="16.5" customHeight="1">
+    <row r="2" spans="1:16" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2287,7 +2487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1">
+    <row r="3" spans="1:16" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2307,7 +2507,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:16" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2327,7 +2527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="16.5" customHeight="1">
+    <row r="5" spans="1:16" ht="16.5" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -2335,17 +2535,17 @@
         <v>20</v>
       </c>
       <c r="C5" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" ht="16.5" customHeight="1">
+    <row r="6" spans="1:16" ht="16.5" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -2353,31 +2553,31 @@
         <v>22</v>
       </c>
       <c r="C6" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" ht="16.5" customHeight="1">
+    <row r="7" spans="1:16" ht="16.5" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" ht="16.5" customHeight="1">
+    <row r="8" spans="1:16" ht="16.5" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -2385,17 +2585,17 @@
         <v>27</v>
       </c>
       <c r="C8" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" ht="16.5" customHeight="1">
+    <row r="9" spans="1:16" ht="16.5" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -2403,15 +2603,15 @@
         <v>29</v>
       </c>
       <c r="C9" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" ht="16.5" customHeight="1">
+    <row r="10" spans="1:16" ht="16.5" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -2419,27 +2619,27 @@
         <v>30</v>
       </c>
       <c r="C10" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" ht="16.5" customHeight="1">
+    <row r="11" spans="1:16" ht="16.5" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" ht="16.5" customHeight="1">
+    <row r="12" spans="1:16" ht="16.5" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -2447,17 +2647,17 @@
         <v>32</v>
       </c>
       <c r="C12" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" ht="16.5" customHeight="1">
+    <row r="13" spans="1:16" ht="16.5" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
@@ -2465,17 +2665,17 @@
         <v>32</v>
       </c>
       <c r="C13" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" ht="16.5" customHeight="1">
+    <row r="14" spans="1:16" ht="16.5" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -2483,19 +2683,19 @@
         <v>33</v>
       </c>
       <c r="C14" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" ht="16.5" customHeight="1">
+    <row r="15" spans="1:16" ht="16.5" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -2503,233 +2703,233 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" ht="16.5" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7" t="s">
+    <row r="16" spans="1:16" ht="16.5" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" ht="16.5" customHeight="1">
-      <c r="A17" s="6" t="s">
+      <c r="C16" s="5">
+        <v>7</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D17" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6" t="s">
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
+        <v>4</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" ht="16.5" customHeight="1">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6">
-        <v>11.0</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6" t="s">
+    <row r="18" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5">
+        <v>11</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" ht="16.5" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7" t="s">
+    <row r="19" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="6">
-        <v>7.0</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" ht="16.5" customHeight="1"/>
-    <row r="21" ht="16.5" customHeight="1"/>
-    <row r="22" ht="16.5" customHeight="1">
-      <c r="B22" s="8"/>
-    </row>
-    <row r="23" ht="16.5" customHeight="1">
-      <c r="B23" s="8"/>
-    </row>
-    <row r="24" ht="16.5" customHeight="1">
-      <c r="B24" s="8"/>
-    </row>
-    <row r="25" ht="16.5" customHeight="1">
-      <c r="B25" s="8"/>
-    </row>
-    <row r="26" ht="16.5" customHeight="1">
-      <c r="B26" s="8"/>
-    </row>
-    <row r="27" ht="16.5" customHeight="1">
-      <c r="B27" s="8"/>
-    </row>
-    <row r="28" ht="16.5" customHeight="1">
-      <c r="B28" s="8"/>
-    </row>
-    <row r="29" ht="16.5" customHeight="1">
-      <c r="B29" s="8"/>
-    </row>
-    <row r="30" ht="16.5" customHeight="1"/>
-    <row r="31" ht="16.5" customHeight="1"/>
-    <row r="32" ht="16.5" customHeight="1">
-      <c r="B32" s="8"/>
-    </row>
-    <row r="33" ht="16.5" customHeight="1"/>
-    <row r="34" ht="16.5" customHeight="1"/>
-    <row r="35" ht="16.5" customHeight="1"/>
-    <row r="36" ht="16.5" customHeight="1"/>
-    <row r="37" ht="16.5" customHeight="1"/>
-    <row r="38" ht="16.5" customHeight="1"/>
-    <row r="39" ht="16.5" customHeight="1"/>
-    <row r="40" ht="16.5" customHeight="1"/>
-    <row r="41" ht="16.5" customHeight="1"/>
-    <row r="42" ht="16.5" customHeight="1"/>
-    <row r="43" ht="16.5" customHeight="1"/>
-    <row r="44" ht="16.5" customHeight="1"/>
-    <row r="45" ht="16.5" customHeight="1"/>
-    <row r="46" ht="16.5" customHeight="1"/>
-    <row r="47" ht="16.5" customHeight="1">
-      <c r="A47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="8"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="8"/>
-      <c r="Q47" s="8"/>
-      <c r="R47" s="8"/>
-      <c r="S47" s="8"/>
-      <c r="T47" s="8"/>
-      <c r="U47" s="8"/>
-      <c r="V47" s="8"/>
-      <c r="W47" s="8"/>
-      <c r="X47" s="8"/>
-      <c r="Y47" s="8"/>
-      <c r="Z47" s="8"/>
-    </row>
-    <row r="48" ht="16.5" customHeight="1">
-      <c r="A48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
-      <c r="R48" s="8"/>
-      <c r="S48" s="8"/>
-      <c r="T48" s="8"/>
-      <c r="U48" s="8"/>
-      <c r="V48" s="8"/>
-      <c r="W48" s="8"/>
-      <c r="X48" s="8"/>
-      <c r="Y48" s="8"/>
-      <c r="Z48" s="8"/>
-    </row>
-    <row r="49" ht="16.5" customHeight="1">
-      <c r="B49" s="8"/>
-    </row>
-    <row r="50" ht="16.5" customHeight="1">
-      <c r="B50" s="8"/>
-    </row>
-    <row r="51" ht="16.5" customHeight="1">
-      <c r="B51" s="8"/>
-    </row>
-    <row r="52" ht="16.5" customHeight="1">
-      <c r="B52" s="8"/>
-    </row>
-    <row r="53" ht="16.5" customHeight="1">
-      <c r="B53" s="8"/>
-    </row>
-    <row r="54" ht="16.5" customHeight="1">
-      <c r="B54" s="8"/>
-    </row>
-    <row r="55" ht="16.5" customHeight="1">
-      <c r="B55" s="8"/>
-    </row>
-    <row r="56" ht="16.5" customHeight="1">
-      <c r="B56" s="8"/>
-    </row>
-    <row r="57" ht="16.5" customHeight="1">
-      <c r="B57" s="8"/>
-    </row>
-    <row r="58" ht="16.5" customHeight="1">
-      <c r="B58" s="8"/>
-    </row>
-    <row r="59" ht="16.5" customHeight="1">
-      <c r="B59" s="8"/>
-    </row>
-    <row r="60" ht="16.5" customHeight="1">
-      <c r="B60" s="8"/>
-    </row>
-    <row r="61" ht="16.5" customHeight="1">
-      <c r="B61" s="8"/>
-    </row>
-    <row r="62" ht="16.5" customHeight="1">
-      <c r="B62" s="8"/>
-    </row>
-    <row r="63" ht="16.5" customHeight="1">
-      <c r="B63" s="8"/>
-    </row>
-    <row r="64" ht="16.5" customHeight="1"/>
-    <row r="65" ht="16.5" customHeight="1"/>
-    <row r="66" ht="16.5" customHeight="1">
-      <c r="B66" s="8"/>
-    </row>
-    <row r="67" ht="16.5" customHeight="1">
-      <c r="B67" s="8"/>
-    </row>
-    <row r="68" ht="16.5" customHeight="1">
-      <c r="B68" s="8"/>
-    </row>
-    <row r="69" ht="16.5" customHeight="1"/>
-    <row r="70" ht="16.5" customHeight="1"/>
-    <row r="71" ht="16.5" customHeight="1">
-      <c r="B71" s="8"/>
-    </row>
-    <row r="72" ht="16.5" customHeight="1">
-      <c r="B72" s="8"/>
-    </row>
-    <row r="73" ht="16.5" customHeight="1">
-      <c r="B73" s="8"/>
-    </row>
-    <row r="74" ht="16.5" customHeight="1"/>
-    <row r="75" ht="16.5" customHeight="1"/>
-    <row r="76" ht="16.5" customHeight="1"/>
-    <row r="77" ht="16.5" customHeight="1"/>
-    <row r="78" ht="16.5" customHeight="1"/>
-    <row r="79" ht="16.5" customHeight="1"/>
-    <row r="80" ht="16.5" customHeight="1"/>
+      <c r="C19" s="5">
+        <v>7</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="21" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="22" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="31" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="32" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="34" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="35" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="36" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="37" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="38" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="39" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="40" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="41" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="42" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="43" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="44" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="45" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="46" spans="1:26" ht="16.5" customHeight="1"/>
+    <row r="47" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
+      <c r="S47" s="7"/>
+      <c r="T47" s="7"/>
+      <c r="U47" s="7"/>
+      <c r="V47" s="7"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="7"/>
+      <c r="Y47" s="7"/>
+      <c r="Z47" s="7"/>
+    </row>
+    <row r="48" spans="1:26" ht="16.5" customHeight="1">
+      <c r="A48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
+      <c r="S48" s="7"/>
+      <c r="T48" s="7"/>
+      <c r="U48" s="7"/>
+      <c r="V48" s="7"/>
+      <c r="W48" s="7"/>
+      <c r="X48" s="7"/>
+      <c r="Y48" s="7"/>
+      <c r="Z48" s="7"/>
+    </row>
+    <row r="49" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B49" s="7"/>
+    </row>
+    <row r="50" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B50" s="7"/>
+    </row>
+    <row r="51" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B51" s="7"/>
+    </row>
+    <row r="52" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B52" s="7"/>
+    </row>
+    <row r="53" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B53" s="7"/>
+    </row>
+    <row r="54" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B54" s="7"/>
+    </row>
+    <row r="55" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B55" s="7"/>
+    </row>
+    <row r="56" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B56" s="7"/>
+    </row>
+    <row r="57" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B57" s="7"/>
+    </row>
+    <row r="58" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B58" s="7"/>
+    </row>
+    <row r="59" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B59" s="7"/>
+    </row>
+    <row r="60" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B60" s="7"/>
+    </row>
+    <row r="61" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B61" s="7"/>
+    </row>
+    <row r="62" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B62" s="7"/>
+    </row>
+    <row r="63" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B63" s="7"/>
+    </row>
+    <row r="64" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="65" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="66" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B66" s="7"/>
+    </row>
+    <row r="67" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B67" s="7"/>
+    </row>
+    <row r="68" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B68" s="7"/>
+    </row>
+    <row r="69" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="70" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="71" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B71" s="7"/>
+    </row>
+    <row r="72" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B72" s="7"/>
+    </row>
+    <row r="73" spans="2:2" ht="16.5" customHeight="1">
+      <c r="B73" s="7"/>
+    </row>
+    <row r="74" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="75" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="76" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="77" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="78" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="79" spans="2:2" ht="16.5" customHeight="1"/>
+    <row r="80" spans="2:2" ht="16.5" customHeight="1"/>
     <row r="81" ht="16.5" customHeight="1"/>
     <row r="82" ht="16.5" customHeight="1"/>
     <row r="83" ht="16.5" customHeight="1"/>
@@ -3651,39 +3851,38 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="11.0"/>
-    <col customWidth="1" min="2" max="2" width="70.43"/>
-    <col customWidth="1" min="3" max="3" width="16.14"/>
-    <col customWidth="1" min="4" max="4" width="18.14"/>
-    <col customWidth="1" min="5" max="5" width="15.43"/>
-    <col customWidth="1" min="6" max="6" width="51.43"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="70.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" ht="16.5" customHeight="1">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3703,7 +3902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -3723,7 +3922,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -3743,442 +3942,442 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="16.5" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9" t="s">
+      <c r="C5" s="8">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" ht="16.5" customHeight="1">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9" t="s">
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" ht="16.5" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A7" s="10"/>
+      <c r="B7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9" t="s">
+      <c r="C7" s="8">
+        <v>6</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" ht="16.5" customHeight="1">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" ht="16.5" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9" t="s">
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9" t="s">
+      <c r="C9" s="8">
+        <v>6</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" ht="16.5" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9">
-        <v>11.0</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9" t="s">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8">
+        <v>11</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" ht="16.5" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9" t="s">
+      <c r="C11" s="8">
+        <v>6</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" ht="16.5" customHeight="1">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" ht="16.5" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="C12" s="8">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A13" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" ht="16.5" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10" t="s">
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9" t="s">
+      <c r="C14" s="8">
+        <v>6</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" ht="16.5" customHeight="1">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" ht="16.5" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10" t="s">
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9" t="s">
+      <c r="C16" s="8">
+        <v>6</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" ht="16.5" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10" t="s">
+    <row r="17" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9" t="s">
+      <c r="C17" s="8">
+        <v>6</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" ht="16.5" customHeight="1">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A18" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D18" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9" t="s">
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8">
+        <v>6</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" ht="16.5" customHeight="1">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D19" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9" t="s">
+      <c r="C19" s="8">
+        <v>1</v>
+      </c>
+      <c r="D19" s="8">
+        <v>4</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" ht="16.5" customHeight="1">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D20" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" ht="16.5" customHeight="1">
-      <c r="A21" s="9" t="s">
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8">
+        <v>6</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D21" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" ht="16.5" customHeight="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10" t="s">
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+      <c r="D21" s="8">
+        <v>4</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9" t="s">
+      <c r="C22" s="8">
+        <v>2</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A23" s="8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" ht="16.5" customHeight="1">
-      <c r="A23" s="9" t="s">
+      <c r="B23" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="C23" s="8">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-    </row>
-    <row r="24" ht="16.5" customHeight="1">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="8">
+        <v>2</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A25" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9" t="s">
+      <c r="C25" s="8">
+        <v>1</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="8">
+        <v>3</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A27" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A28" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" ht="16.5" customHeight="1">
-      <c r="A25" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="10" t="s">
+      <c r="C28" s="8">
+        <v>1</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A29" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" ht="16.5" customHeight="1">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="9">
-        <v>3.0</v>
-      </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" ht="16.5" customHeight="1">
-      <c r="A27" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" ht="16.5" customHeight="1">
-      <c r="A28" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="10" t="s">
+      <c r="C29" s="8">
+        <v>1</v>
+      </c>
+      <c r="D29" s="8">
+        <v>6</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8">
+        <v>11</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-    </row>
-    <row r="29" ht="16.5" customHeight="1">
-      <c r="A29" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="9" t="s">
+      <c r="C31" s="8">
+        <v>7</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D29" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" ht="16.5" customHeight="1">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9">
-        <v>11.0</v>
-      </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" ht="16.5" customHeight="1">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9" t="s">
+      <c r="C32" s="8">
+        <v>11</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8">
+        <v>5</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="9">
-        <v>7.0</v>
-      </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32" ht="16.5" customHeight="1">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="9">
-        <v>11.0</v>
-      </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" ht="16.5" customHeight="1">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9">
-        <v>5.0</v>
-      </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" ht="16.5" customHeight="1">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" ht="16.5" customHeight="1"/>
-    <row r="36" ht="16.5" customHeight="1"/>
-    <row r="37" ht="16.5" customHeight="1"/>
-    <row r="38" ht="16.5" customHeight="1"/>
-    <row r="39" ht="16.5" customHeight="1"/>
-    <row r="40" ht="16.5" customHeight="1"/>
-    <row r="41" ht="16.5" customHeight="1"/>
-    <row r="42" ht="16.5" customHeight="1"/>
-    <row r="43" ht="16.5" customHeight="1"/>
-    <row r="44" ht="16.5" customHeight="1"/>
-    <row r="45" ht="16.5" customHeight="1"/>
-    <row r="46" ht="16.5" customHeight="1"/>
-    <row r="47" ht="16.5" customHeight="1"/>
-    <row r="48" ht="16.5" customHeight="1"/>
+      <c r="C34" s="8">
+        <v>4</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="36" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="37" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="38" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="39" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="40" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="41" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="42" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="43" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="44" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="45" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="46" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="47" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="48" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="49" ht="16.5" customHeight="1"/>
     <row r="50" ht="16.5" customHeight="1"/>
     <row r="51" ht="16.5" customHeight="1"/>
@@ -5132,38 +5331,35 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.43"/>
-    <col customWidth="1" min="2" max="2" width="59.14"/>
-    <col customWidth="1" min="3" max="4" width="25.0"/>
-    <col customWidth="1" min="5" max="5" width="21.43"/>
-    <col customWidth="1" min="6" max="6" width="9.57"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" customWidth="1"/>
+    <col min="3" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" ht="16.5" customHeight="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -5183,7 +5379,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -5203,7 +5399,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -5223,80 +5419,80 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="16.5" customHeight="1">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" ht="16.5" customHeight="1">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" ht="16.5" customHeight="1">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="8" ht="16.5" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C8" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9" ht="16.5" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="C9" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" ht="16.5" customHeight="1"/>
-    <row r="11" ht="16.5" customHeight="1"/>
-    <row r="12" ht="16.5" customHeight="1"/>
-    <row r="13" ht="16.5" customHeight="1"/>
-    <row r="14" ht="16.5" customHeight="1"/>
-    <row r="15" ht="16.5" customHeight="1"/>
-    <row r="16" ht="16.5" customHeight="1"/>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="11" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="15" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="17" ht="16.5" customHeight="1"/>
     <row r="18" ht="16.5" customHeight="1"/>
     <row r="19" ht="16.5" customHeight="1"/>
@@ -6282,43 +6478,40 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.43"/>
-    <col customWidth="1" min="2" max="2" width="29.14"/>
-    <col customWidth="1" min="3" max="4" width="25.0"/>
-    <col customWidth="1" min="5" max="5" width="21.43"/>
-    <col customWidth="1" min="6" max="6" width="9.57"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="3" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
-      <c r="A1" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" ht="16.5" customHeight="1">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6338,7 +6531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -6358,7 +6551,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -6378,55 +6571,55 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="16.5" customHeight="1">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" ht="16.5" customHeight="1">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" ht="16.5" customHeight="1">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="8" ht="16.5" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -6434,13 +6627,13 @@
         <v>32</v>
       </c>
       <c r="C8" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="9" ht="16.5" customHeight="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -6448,36 +6641,36 @@
         <v>32</v>
       </c>
       <c r="C9" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="10" ht="16.5" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C10" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="11" ht="16.5" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="C11" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" ht="16.5" customHeight="1"/>
-    <row r="13" ht="16.5" customHeight="1"/>
-    <row r="14" ht="16.5" customHeight="1"/>
-    <row r="15" ht="16.5" customHeight="1"/>
-    <row r="16" ht="16.5" customHeight="1"/>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="15" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="17" ht="16.5" customHeight="1"/>
     <row r="18" ht="16.5" customHeight="1"/>
     <row r="19" ht="16.5" customHeight="1"/>
@@ -7463,43 +7656,40 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.43"/>
-    <col customWidth="1" min="2" max="2" width="24.43"/>
-    <col customWidth="1" min="3" max="4" width="25.0"/>
-    <col customWidth="1" min="5" max="5" width="21.43"/>
-    <col customWidth="1" min="6" max="6" width="9.57"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
-      <c r="A1" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" ht="16.5" customHeight="1">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7519,7 +7709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -7539,7 +7729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="16.5" customHeight="1">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -7559,51 +7749,51 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="16.5" customHeight="1">
+    <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" ht="16.5" customHeight="1">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C6" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7" ht="16.5" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" customHeight="1">
       <c r="C7" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" ht="16.5" customHeight="1"/>
-    <row r="9" ht="16.5" customHeight="1"/>
-    <row r="10" ht="16.5" customHeight="1"/>
-    <row r="11" ht="16.5" customHeight="1"/>
-    <row r="12" ht="16.5" customHeight="1"/>
-    <row r="13" ht="16.5" customHeight="1"/>
-    <row r="14" ht="16.5" customHeight="1"/>
-    <row r="15" ht="16.5" customHeight="1"/>
-    <row r="16" ht="16.5" customHeight="1"/>
+    <row r="8" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="11" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="15" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="17" ht="16.5" customHeight="1"/>
     <row r="18" ht="16.5" customHeight="1"/>
     <row r="19" ht="16.5" customHeight="1"/>
@@ -8589,10 +8779,9 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>